<commit_message>
WIP (Dummy-Funktion geht schon)
</commit_message>
<xml_diff>
--- a/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48FF2E0-994A-48F3-8AAE-A36D3AD84A65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C568388-E20A-4A8A-8318-DBE7645D1702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,6 +245,24 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
+  </si>
+  <si>
+    <t>Guessed License URL</t>
+  </si>
+  <si>
+    <t>Guessed License URL AuditInfo</t>
+  </si>
+  <si>
+    <t>Guessed License URL Text</t>
+  </si>
+  <si>
+    <t>$guessedLicenseUrl$</t>
+  </si>
+  <si>
+    <t>$guessedLicenseUrlAuditInfo$</t>
+  </si>
+  <si>
+    <t>$guessedLicenseContent$</t>
   </si>
 </sst>
 </file>
@@ -283,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +389,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -420,6 +450,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,22 +734,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -725,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
@@ -733,8 +765,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
@@ -748,7 +780,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -762,7 +794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -776,7 +808,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -790,7 +822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -810,7 +842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,7 +862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -843,34 +875,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="8" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="8" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.54296875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.7265625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.54296875" style="6" customWidth="1"/>
+    <col min="14" max="16" width="31.54296875" style="22" customWidth="1"/>
+    <col min="17" max="17" width="20.453125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="20.1796875" style="7" customWidth="1"/>
+    <col min="19" max="19" width="29.54296875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="17.7265625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="19.54296875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -910,26 +943,35 @@
       <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -969,22 +1011,31 @@
       <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Alternative Reports mit guessedLicense
</commit_message>
<xml_diff>
--- a/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C568388-E20A-4A8A-8318-DBE7645D1702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B43F4-6420-4D77-9BAE-981EA2068EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -253,16 +253,10 @@
     <t>Guessed License URL AuditInfo</t>
   </si>
   <si>
-    <t>Guessed License URL Text</t>
-  </si>
-  <si>
     <t>$guessedLicenseUrl$</t>
   </si>
   <si>
     <t>$guessedLicenseUrlAuditInfo$</t>
-  </si>
-  <si>
-    <t>$guessedLicenseContent$</t>
   </si>
 </sst>
 </file>
@@ -875,10 +869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,16 +888,16 @@
     <col min="10" max="10" width="23.1796875" style="5" customWidth="1"/>
     <col min="11" max="12" width="28.7265625" style="6" customWidth="1"/>
     <col min="13" max="13" width="31.54296875" style="6" customWidth="1"/>
-    <col min="14" max="16" width="31.54296875" style="22" customWidth="1"/>
-    <col min="17" max="17" width="20.453125" style="7" customWidth="1"/>
-    <col min="18" max="18" width="20.1796875" style="7" customWidth="1"/>
-    <col min="19" max="19" width="29.54296875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="17.7265625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="19.54296875" style="8" customWidth="1"/>
-    <col min="22" max="22" width="19.54296875" style="1" customWidth="1"/>
+    <col min="14" max="15" width="31.54296875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="20.453125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="20.1796875" style="7" customWidth="1"/>
+    <col min="18" max="18" width="29.54296875" style="4" customWidth="1"/>
+    <col min="19" max="19" width="17.7265625" style="8" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" style="8" customWidth="1"/>
+    <col min="21" max="21" width="19.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -949,29 +943,26 @@
       <c r="O1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="P1" s="23" t="s">
-        <v>73</v>
+      <c r="P1" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="S1" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="T1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1012,30 +1003,27 @@
         <v>35</v>
       </c>
       <c r="N2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>76</v>
+      <c r="P2" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="S2" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="T2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature license guessing (#90)
Co-authored-by: Philip Garus <philip.garus@capgemini.com>
Co-authored-by: pgarus <35223024+pgarus97@users.noreply.github.com>
Co-authored-by: Dung Pham <dung.a.pham@capgemini.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/com/devonfw/tools/solicitor/templates/Solicitor_Output_Template_Sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48FF2E0-994A-48F3-8AAE-A36D3AD84A65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B43F4-6420-4D77-9BAE-981EA2068EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>#MODELROOT#$extensionBuilddate$</t>
+  </si>
+  <si>
+    <t>Guessed License URL</t>
+  </si>
+  <si>
+    <t>Guessed License URL AuditInfo</t>
+  </si>
+  <si>
+    <t>$guessedLicenseUrl$</t>
+  </si>
+  <si>
+    <t>$guessedLicenseUrlAuditInfo$</t>
   </si>
 </sst>
 </file>
@@ -283,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -420,6 +444,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,22 +728,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -725,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
@@ -733,8 +759,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
@@ -748,7 +774,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -762,7 +788,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -776,7 +802,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -790,7 +816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -810,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,7 +856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -843,34 +869,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="4" customWidth="1"/>
     <col min="5" max="5" width="26" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="18.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="28.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="8" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="8" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.54296875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.7265625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.54296875" style="6" customWidth="1"/>
+    <col min="14" max="15" width="31.54296875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="20.453125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="20.1796875" style="7" customWidth="1"/>
+    <col min="18" max="18" width="29.54296875" style="4" customWidth="1"/>
+    <col min="19" max="19" width="17.7265625" style="8" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" style="8" customWidth="1"/>
+    <col min="21" max="21" width="19.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
@@ -910,26 +937,32 @@
       <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -969,22 +1002,28 @@
       <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>